<commit_message>
EDA oppdatert. Muligens rekkefølge skal endres
</commit_message>
<xml_diff>
--- a/Machine-Learning-Features.xlsx
+++ b/Machine-Learning-Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60fb636958e87b31/Dokumenter/UNI/2023 Autumn/TDT4173 Machine Learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive - NTNU\Documents\NTNU_studier\11.semester(YOLO)\TDT4173-Machine-Learning-Solar-Energy-Production-Forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{F5EAFB1F-273F-443C-881C-B9035403A0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A458F16C-AFDF-4024-BF92-8D82D906B9D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BA1A28-4330-4E09-95BA-9BCF747A2942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13110" yWindow="0" windowWidth="6180" windowHeight="10170" xr2:uid="{30A50CEF-CA50-4B27-B3F6-2E64D76A551D}"/>
+    <workbookView xWindow="30450" yWindow="1650" windowWidth="21600" windowHeight="11175" xr2:uid="{30A50CEF-CA50-4B27-B3F6-2E64D76A551D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -85,13 +85,88 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>snow_density:kgm3</t>
+  </si>
+  <si>
+    <t>snow_depth:cm</t>
+  </si>
+  <si>
+    <t>snow_drift:idx</t>
+  </si>
+  <si>
+    <t>snow_melt_10min:mm</t>
+  </si>
+  <si>
+    <t>A Pred</t>
+  </si>
+  <si>
+    <t>Pred A</t>
+  </si>
+  <si>
+    <t>fresh_snow_12h:cm</t>
+  </si>
+  <si>
+    <t>fresh_snow_1h:cm</t>
+  </si>
+  <si>
+    <t>fresh_snow_24h:cm</t>
+  </si>
+  <si>
+    <t>fresh_snow_3h:cm</t>
+  </si>
+  <si>
+    <t>fresh_snow_6h:cm</t>
+  </si>
+  <si>
+    <t>prob_rime:p</t>
+  </si>
+  <si>
+    <t>Mostly 0 or constant:</t>
+  </si>
+  <si>
+    <t>snow_water:kgm2</t>
+  </si>
+  <si>
+    <t>direct_rad</t>
+  </si>
+  <si>
+    <t>diffuse_rad:W</t>
+  </si>
+  <si>
+    <t>Looks wery usefull</t>
+  </si>
+  <si>
+    <t>rad ++</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Snow for B not awefull</t>
+  </si>
+  <si>
+    <t>is_day</t>
+  </si>
+  <si>
+    <t>is_shadow</t>
+  </si>
+  <si>
+    <t>categorial</t>
+  </si>
+  <si>
+    <t>Pred B</t>
+  </si>
+  <si>
+    <t>constant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +177,12 @@
     <font>
       <sz val="7"/>
       <color rgb="FF292929"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCCCCCC"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -126,9 +207,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,15 +525,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC964312-49AB-47C6-9BFB-D18EC06E9068}">
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.08984375" customWidth="1"/>
+    <col min="2" max="2" width="26.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -586,7 +668,262 @@
         <v>19</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>